<commit_message>
Add support for nullables
</commit_message>
<xml_diff>
--- a/src/ExcelMapper.Tests/Resources/EmptyValues.xlsx
+++ b/src/ExcelMapper.Tests/Resources/EmptyValues.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>IntValue</t>
   </si>
@@ -39,6 +39,18 @@
   </si>
   <si>
     <t>DateValue</t>
+  </si>
+  <si>
+    <t>ArrayValue1</t>
+  </si>
+  <si>
+    <t>ArrayValue2</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -74,8 +86,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -356,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -376,7 +389,7 @@
     <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -392,22 +405,34 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1">
+        <v>42921</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
         <v>2</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>4</v>
-      </c>
-      <c r="E3">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>